<commit_message>
completed the second exercice of the project
the project is completed
</commit_message>
<xml_diff>
--- a/Finals Project/data/exercice2.xlsx
+++ b/Finals Project/data/exercice2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\License Big Data\Semester 5\Techniques de prevision\notebooks\Finals Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9F582F-881A-4F02-876B-8AC0069DB2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949D93FD-4B55-4DBF-993F-CF8390936B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="3240" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
     <t>Continente</t>
   </si>
   <si>
-    <t>Dis Mag Value</t>
+    <t>Dis_Mag_Value</t>
   </si>
   <si>
-    <t>nombre total de décès</t>
+    <t>nombre_total_de_deces</t>
   </si>
   <si>
-    <t>Total Affecté</t>
+    <t>Total_des_dommages</t>
   </si>
   <si>
-    <t>Total des dommages ('000 US $)</t>
+    <t>Total_Affecte</t>
   </si>
 </sst>
 </file>
@@ -99,10 +99,10 @@
   <autoFilter ref="A1:E109" xr:uid="{8E31F5E8-12AC-4CB4-B286-1084C31765CE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{795D6CA8-914B-4EB5-95FB-3C8B695F7B0A}" name="Continente"/>
-    <tableColumn id="2" xr3:uid="{331231EC-B0B1-4320-8B7D-76F7D2A9C232}" name="Dis Mag Value"/>
-    <tableColumn id="3" xr3:uid="{A5D3E322-32B6-479E-A24E-8E59401A935B}" name="nombre total de décès"/>
-    <tableColumn id="4" xr3:uid="{3224EDED-EAEF-47BE-AB55-08DC034D4B37}" name="Total Affecté"/>
-    <tableColumn id="5" xr3:uid="{4E8A4D6A-C097-44E4-8127-8D1FAAFE4631}" name="Total des dommages ('000 US $)"/>
+    <tableColumn id="2" xr3:uid="{331231EC-B0B1-4320-8B7D-76F7D2A9C232}" name="Dis_Mag_Value"/>
+    <tableColumn id="3" xr3:uid="{A5D3E322-32B6-479E-A24E-8E59401A935B}" name="nombre_total_de_deces"/>
+    <tableColumn id="4" xr3:uid="{3224EDED-EAEF-47BE-AB55-08DC034D4B37}" name="Total_Affecte"/>
+    <tableColumn id="5" xr3:uid="{4E8A4D6A-C097-44E4-8127-8D1FAAFE4631}" name="Total_des_dommages"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,9 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -455,10 +453,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>